<commit_message>
adding rhino watch analysis
</commit_message>
<xml_diff>
--- a/Eric/Outlier detection/weights.xlsx
+++ b/Eric/Outlier detection/weights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudentsITeach\Eric\Outlier detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Music\StudentsWork-Lessons-\Eric\Outlier detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E08C0E-3DF8-4369-94E0-8E87A2291A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B68DAA-4340-47A3-82B1-300733C6B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{135B6ED4-E062-4A0C-BA8F-63107FC657C2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{135B6ED4-E062-4A0C-BA8F-63107FC657C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Weight</t>
   </si>
@@ -60,6 +49,9 @@
   </si>
   <si>
     <t>OUTLIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -414,16 +406,16 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>16</v>
       </c>
@@ -482,25 +474,28 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>42</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B10" si="0">IF(OR(A3&lt;$H$2,A3&gt;$I$2),"OUTLIER","NORMAL")</f>
-        <v>NORMAL</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f>IF(OR(A3&lt;$H$2,A3&gt;$I$2),"OUTLIER","NORMAL")</f>
+        <v>NORMAL</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>53</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>NORMAL</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B3:B10" si="0">IF(OR(A4&lt;$H$2,A4&gt;$I$2),"OUTLIER","NORMAL")</f>
+        <v>NORMAL</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>61</v>
       </c>
@@ -509,7 +504,7 @@
         <v>NORMAL</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>68</v>
       </c>
@@ -518,7 +513,7 @@
         <v>NORMAL</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>69</v>
       </c>
@@ -527,7 +522,7 @@
         <v>NORMAL</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>71</v>
       </c>
@@ -536,7 +531,7 @@
         <v>NORMAL</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>76</v>
       </c>
@@ -544,8 +539,11 @@
         <f t="shared" si="0"/>
         <v>NORMAL</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>130</v>
       </c>

</xml_diff>